<commit_message>
Added master regions, optimised price solver, added fixed tariff logic
</commit_message>
<xml_diff>
--- a/gasmarketmodel/data/outputs/Master.xlsx
+++ b/gasmarketmodel/data/outputs/Master.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario" sheetId="1" state="visible" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="LNG" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="Connections" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="Price" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Mapping" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="D_CONNECTION_NAME" localSheetId="6">OFFSET(Connections!$A$18,0,0,COUNTA(Connections!$A$18:$A$116))</definedName>
@@ -5704,7 +5705,7 @@
   </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -5987,177 +5988,177 @@
     <row r="6">
       <c r="A6" s="4" t="inlineStr">
         <is>
-          <t>Deutschland</t>
+          <t>Benelux</t>
         </is>
       </c>
       <c r="B6" s="6" t="n">
         <v>5</v>
       </c>
       <c r="C6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="D6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="E6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="F6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="G6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="H6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="I6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="J6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="K6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="L6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="M6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="N6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="O6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="P6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="Q6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="R6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="S6" s="2" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="4" t="inlineStr">
         <is>
-          <t>Frankreich</t>
+          <t>Deutschland</t>
         </is>
       </c>
       <c r="B7" s="6" t="n">
         <v>5</v>
       </c>
       <c r="C7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="D7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="E7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="F7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="G7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="H7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="I7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="J7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="K7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="L7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="M7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="N7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="O7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="P7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="Q7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="R7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="S7" s="2" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="4" t="inlineStr">
         <is>
-          <t>Niederlande</t>
+          <t>Frankreich</t>
         </is>
       </c>
       <c r="B8" s="6" t="n">
         <v>5</v>
       </c>
       <c r="C8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="D8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="E8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="F8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="G8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="H8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="I8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="J8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="K8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="L8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="M8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="N8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="O8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="P8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="Q8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="R8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="S8" s="2" t="n"/>
     </row>
@@ -6171,52 +6172,52 @@
         <v>8</v>
       </c>
       <c r="C9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="D9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="E9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="F9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="G9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="H9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="I9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="J9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="K9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="L9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="M9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="N9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="O9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="P9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="Q9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="R9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="S9" s="2" t="n"/>
     </row>
@@ -8521,177 +8522,177 @@
     <row r="6">
       <c r="A6" s="4" t="inlineStr">
         <is>
-          <t>Deutschland</t>
+          <t>Benelux</t>
         </is>
       </c>
       <c r="B6" s="6" t="n">
         <v>2</v>
       </c>
       <c r="C6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="D6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="E6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="F6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="G6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="H6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="I6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="J6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="K6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="L6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="M6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="N6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="O6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="P6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="Q6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="R6" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="S6" s="2" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="4" t="inlineStr">
         <is>
-          <t>Frankreich</t>
+          <t>Deutschland</t>
         </is>
       </c>
       <c r="B7" s="6" t="n">
         <v>2</v>
       </c>
       <c r="C7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="D7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="E7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="F7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="G7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="H7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="I7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="J7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="K7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="L7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="M7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="N7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="O7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="P7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="Q7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="R7" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="S7" s="2" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="4" t="inlineStr">
         <is>
-          <t>Niederlande</t>
+          <t>Frankreich</t>
         </is>
       </c>
       <c r="B8" s="6" t="n">
         <v>2</v>
       </c>
       <c r="C8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="D8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="E8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="F8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="G8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="H8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="I8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="J8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="K8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="L8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="M8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="N8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="O8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="P8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="Q8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="R8" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="S8" s="2" t="n"/>
     </row>
@@ -8705,52 +8706,52 @@
         <v>9</v>
       </c>
       <c r="C9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="D9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="E9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="F9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="G9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="H9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="I9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="J9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="K9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="L9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="M9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="N9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="O9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="P9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="Q9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="R9" s="6" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="S9" s="2" t="n"/>
     </row>
@@ -11578,7 +11579,7 @@
     <row r="16">
       <c r="A16" s="4" t="inlineStr">
         <is>
-          <t>Deutschland</t>
+          <t>Benelux</t>
         </is>
       </c>
       <c r="B16" s="4" t="inlineStr">
@@ -11610,7 +11611,7 @@
     <row r="17">
       <c r="A17" s="4" t="inlineStr">
         <is>
-          <t>Deutschland</t>
+          <t>Benelux</t>
         </is>
       </c>
       <c r="B17" s="4" t="inlineStr">
@@ -11619,7 +11620,7 @@
         </is>
       </c>
       <c r="C17" s="6" t="n">
-        <v>-3</v>
+        <v>-0</v>
       </c>
       <c r="D17" s="6" t="n"/>
       <c r="E17" s="6" t="n"/>
@@ -11642,7 +11643,7 @@
     <row r="18">
       <c r="A18" s="4" t="inlineStr">
         <is>
-          <t>Deutschland</t>
+          <t>Benelux</t>
         </is>
       </c>
       <c r="B18" s="4" t="inlineStr">
@@ -11651,7 +11652,7 @@
         </is>
       </c>
       <c r="C18" s="6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D18" s="6" t="n"/>
       <c r="E18" s="6" t="n"/>
@@ -11674,7 +11675,7 @@
     <row r="19">
       <c r="A19" s="4" t="inlineStr">
         <is>
-          <t>Deutschland</t>
+          <t>Benelux</t>
         </is>
       </c>
       <c r="B19" s="4" t="inlineStr">
@@ -11683,7 +11684,7 @@
         </is>
       </c>
       <c r="C19" s="6" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D19" s="6" t="n"/>
       <c r="E19" s="6" t="n"/>
@@ -11706,7 +11707,7 @@
     <row r="20">
       <c r="A20" s="4" t="inlineStr">
         <is>
-          <t>Deutschland</t>
+          <t>Benelux</t>
         </is>
       </c>
       <c r="B20" s="4" t="inlineStr">
@@ -11715,7 +11716,7 @@
         </is>
       </c>
       <c r="C20" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="6" t="n"/>
       <c r="E20" s="6" t="n"/>
@@ -11738,7 +11739,7 @@
     <row r="21">
       <c r="A21" s="4" t="inlineStr">
         <is>
-          <t>Deutschland</t>
+          <t>Benelux</t>
         </is>
       </c>
       <c r="B21" s="4" t="inlineStr">
@@ -11770,7 +11771,7 @@
     <row r="22">
       <c r="A22" s="4" t="inlineStr">
         <is>
-          <t>Frankreich</t>
+          <t>Deutschland</t>
         </is>
       </c>
       <c r="B22" s="4" t="inlineStr">
@@ -11802,7 +11803,7 @@
     <row r="23">
       <c r="A23" s="4" t="inlineStr">
         <is>
-          <t>Frankreich</t>
+          <t>Deutschland</t>
         </is>
       </c>
       <c r="B23" s="4" t="inlineStr">
@@ -11811,7 +11812,7 @@
         </is>
       </c>
       <c r="C23" s="6" t="n">
-        <v>-0</v>
+        <v>-3</v>
       </c>
       <c r="D23" s="6" t="n"/>
       <c r="E23" s="6" t="n"/>
@@ -11834,7 +11835,7 @@
     <row r="24">
       <c r="A24" s="4" t="inlineStr">
         <is>
-          <t>Frankreich</t>
+          <t>Deutschland</t>
         </is>
       </c>
       <c r="B24" s="4" t="inlineStr">
@@ -11843,7 +11844,7 @@
         </is>
       </c>
       <c r="C24" s="6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D24" s="6" t="n"/>
       <c r="E24" s="6" t="n"/>
@@ -11866,7 +11867,7 @@
     <row r="25">
       <c r="A25" s="4" t="inlineStr">
         <is>
-          <t>Frankreich</t>
+          <t>Deutschland</t>
         </is>
       </c>
       <c r="B25" s="4" t="inlineStr">
@@ -11875,7 +11876,7 @@
         </is>
       </c>
       <c r="C25" s="6" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D25" s="6" t="n"/>
       <c r="E25" s="6" t="n"/>
@@ -11898,7 +11899,7 @@
     <row r="26">
       <c r="A26" s="4" t="inlineStr">
         <is>
-          <t>Frankreich</t>
+          <t>Deutschland</t>
         </is>
       </c>
       <c r="B26" s="4" t="inlineStr">
@@ -11907,7 +11908,7 @@
         </is>
       </c>
       <c r="C26" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" s="6" t="n"/>
       <c r="E26" s="6" t="n"/>
@@ -11930,7 +11931,7 @@
     <row r="27">
       <c r="A27" s="4" t="inlineStr">
         <is>
-          <t>Frankreich</t>
+          <t>Deutschland</t>
         </is>
       </c>
       <c r="B27" s="4" t="inlineStr">
@@ -11962,7 +11963,7 @@
     <row r="28">
       <c r="A28" s="4" t="inlineStr">
         <is>
-          <t>Niederlande</t>
+          <t>Frankreich</t>
         </is>
       </c>
       <c r="B28" s="4" t="inlineStr">
@@ -11994,7 +11995,7 @@
     <row r="29">
       <c r="A29" s="4" t="inlineStr">
         <is>
-          <t>Niederlande</t>
+          <t>Frankreich</t>
         </is>
       </c>
       <c r="B29" s="4" t="inlineStr">
@@ -12026,7 +12027,7 @@
     <row r="30">
       <c r="A30" s="4" t="inlineStr">
         <is>
-          <t>Niederlande</t>
+          <t>Frankreich</t>
         </is>
       </c>
       <c r="B30" s="4" t="inlineStr">
@@ -12058,7 +12059,7 @@
     <row r="31">
       <c r="A31" s="4" t="inlineStr">
         <is>
-          <t>Niederlande</t>
+          <t>Frankreich</t>
         </is>
       </c>
       <c r="B31" s="4" t="inlineStr">
@@ -12090,7 +12091,7 @@
     <row r="32">
       <c r="A32" s="4" t="inlineStr">
         <is>
-          <t>Niederlande</t>
+          <t>Frankreich</t>
         </is>
       </c>
       <c r="B32" s="4" t="inlineStr">
@@ -12122,7 +12123,7 @@
     <row r="33">
       <c r="A33" s="4" t="inlineStr">
         <is>
-          <t>Niederlande</t>
+          <t>Frankreich</t>
         </is>
       </c>
       <c r="B33" s="4" t="inlineStr">
@@ -14016,8 +14017,8 @@
   </sheetPr>
   <dimension ref="A1:U116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -14746,7 +14747,7 @@
     <row r="20">
       <c r="A20" s="4" t="inlineStr">
         <is>
-          <t>Import Nor-DE I</t>
+          <t>Import Nor-NL</t>
         </is>
       </c>
       <c r="B20" s="4" t="inlineStr">
@@ -14756,11 +14757,11 @@
       </c>
       <c r="C20" s="4" t="inlineStr">
         <is>
-          <t>Deutschland</t>
+          <t>Benelux</t>
         </is>
       </c>
       <c r="D20" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="6" t="n"/>
       <c r="F20" s="6" t="n"/>
@@ -14783,7 +14784,7 @@
     <row r="21">
       <c r="A21" s="4" t="inlineStr">
         <is>
-          <t>Import Nor-DE II</t>
+          <t>Import Nor-DE I</t>
         </is>
       </c>
       <c r="B21" s="4" t="inlineStr">
@@ -14820,7 +14821,7 @@
     <row r="22">
       <c r="A22" s="4" t="inlineStr">
         <is>
-          <t>Import Nor-FR</t>
+          <t>Import Nor-DE II</t>
         </is>
       </c>
       <c r="B22" s="4" t="inlineStr">
@@ -14830,7 +14831,7 @@
       </c>
       <c r="C22" s="4" t="inlineStr">
         <is>
-          <t>Frankreich</t>
+          <t>Deutschland</t>
         </is>
       </c>
       <c r="D22" s="6" t="n">
@@ -14857,7 +14858,7 @@
     <row r="23">
       <c r="A23" s="4" t="inlineStr">
         <is>
-          <t>Import Nor-NL</t>
+          <t>Import Nor-FR</t>
         </is>
       </c>
       <c r="B23" s="4" t="inlineStr">
@@ -14867,11 +14868,11 @@
       </c>
       <c r="C23" s="4" t="inlineStr">
         <is>
-          <t>Niederlande</t>
+          <t>Frankreich</t>
         </is>
       </c>
       <c r="D23" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" s="6" t="n"/>
       <c r="F23" s="6" t="n"/>
@@ -17605,7 +17606,7 @@
     <row r="15">
       <c r="A15" s="4" t="inlineStr">
         <is>
-          <t>GATE DE</t>
+          <t>GATE NL</t>
         </is>
       </c>
       <c r="B15" s="4" t="inlineStr">
@@ -17615,11 +17616,11 @@
       </c>
       <c r="C15" s="4" t="inlineStr">
         <is>
-          <t>Deutschland</t>
+          <t>Benelux</t>
         </is>
       </c>
       <c r="D15" s="6" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E15" s="6" t="n"/>
       <c r="F15" s="6" t="n"/>
@@ -17642,7 +17643,7 @@
     <row r="16">
       <c r="A16" s="4" t="inlineStr">
         <is>
-          <t>GATE NL</t>
+          <t>GATE DE</t>
         </is>
       </c>
       <c r="B16" s="4" t="inlineStr">
@@ -17652,11 +17653,11 @@
       </c>
       <c r="C16" s="4" t="inlineStr">
         <is>
-          <t>Niederlande</t>
+          <t>Deutschland</t>
         </is>
       </c>
       <c r="D16" s="6" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E16" s="6" t="n"/>
       <c r="F16" s="6" t="n"/>
@@ -20576,21 +20577,21 @@
     <row r="18">
       <c r="A18" s="4" t="inlineStr">
         <is>
-          <t>DE-FR I</t>
+          <t>NL-DE</t>
         </is>
       </c>
       <c r="B18" s="4" t="inlineStr">
+        <is>
+          <t>Benelux</t>
+        </is>
+      </c>
+      <c r="C18" s="4" t="inlineStr">
         <is>
           <t>Deutschland</t>
         </is>
       </c>
-      <c r="C18" s="4" t="inlineStr">
-        <is>
-          <t>Frankreich</t>
-        </is>
-      </c>
       <c r="D18" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E18" s="6" t="n"/>
       <c r="F18" s="6" t="n"/>
@@ -20613,12 +20614,12 @@
     <row r="19">
       <c r="A19" s="4" t="inlineStr">
         <is>
-          <t>DE-FR II</t>
+          <t>NL-FR</t>
         </is>
       </c>
       <c r="B19" s="4" t="inlineStr">
         <is>
-          <t>Deutschland</t>
+          <t>Benelux</t>
         </is>
       </c>
       <c r="C19" s="4" t="inlineStr">
@@ -20627,7 +20628,7 @@
         </is>
       </c>
       <c r="D19" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E19" s="6" t="n"/>
       <c r="F19" s="6" t="n"/>
@@ -20660,7 +20661,7 @@
       </c>
       <c r="C20" s="4" t="inlineStr">
         <is>
-          <t>Niederlande</t>
+          <t>Benelux</t>
         </is>
       </c>
       <c r="D20" s="6" t="n">
@@ -20687,7 +20688,7 @@
     <row r="21">
       <c r="A21" s="4" t="inlineStr">
         <is>
-          <t>DE-CH</t>
+          <t>DE-FR I</t>
         </is>
       </c>
       <c r="B21" s="4" t="inlineStr">
@@ -20697,11 +20698,11 @@
       </c>
       <c r="C21" s="4" t="inlineStr">
         <is>
-          <t>Schweiz</t>
+          <t>Frankreich</t>
         </is>
       </c>
       <c r="D21" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E21" s="6" t="n"/>
       <c r="F21" s="6" t="n"/>
@@ -20724,21 +20725,21 @@
     <row r="22">
       <c r="A22" s="4" t="inlineStr">
         <is>
-          <t>FR-DE</t>
+          <t>DE-FR II</t>
         </is>
       </c>
       <c r="B22" s="4" t="inlineStr">
+        <is>
+          <t>Deutschland</t>
+        </is>
+      </c>
+      <c r="C22" s="4" t="inlineStr">
         <is>
           <t>Frankreich</t>
         </is>
       </c>
-      <c r="C22" s="4" t="inlineStr">
-        <is>
-          <t>Deutschland</t>
-        </is>
-      </c>
       <c r="D22" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E22" s="6" t="n"/>
       <c r="F22" s="6" t="n"/>
@@ -20761,17 +20762,17 @@
     <row r="23">
       <c r="A23" s="4" t="inlineStr">
         <is>
-          <t>FR-NL</t>
+          <t>DE-CH</t>
         </is>
       </c>
       <c r="B23" s="4" t="inlineStr">
         <is>
-          <t>Frankreich</t>
+          <t>Deutschland</t>
         </is>
       </c>
       <c r="C23" s="4" t="inlineStr">
         <is>
-          <t>Niederlande</t>
+          <t>Schweiz</t>
         </is>
       </c>
       <c r="D23" s="6" t="n">
@@ -20798,7 +20799,7 @@
     <row r="24">
       <c r="A24" s="4" t="inlineStr">
         <is>
-          <t>FR-CH</t>
+          <t>FR-NL</t>
         </is>
       </c>
       <c r="B24" s="4" t="inlineStr">
@@ -20808,7 +20809,7 @@
       </c>
       <c r="C24" s="4" t="inlineStr">
         <is>
-          <t>Schweiz</t>
+          <t>Benelux</t>
         </is>
       </c>
       <c r="D24" s="6" t="n">
@@ -20835,12 +20836,12 @@
     <row r="25">
       <c r="A25" s="4" t="inlineStr">
         <is>
-          <t>NL-DE</t>
+          <t>FR-DE</t>
         </is>
       </c>
       <c r="B25" s="4" t="inlineStr">
         <is>
-          <t>Niederlande</t>
+          <t>Frankreich</t>
         </is>
       </c>
       <c r="C25" s="4" t="inlineStr">
@@ -20872,17 +20873,17 @@
     <row r="26">
       <c r="A26" s="4" t="inlineStr">
         <is>
-          <t>NL-FR</t>
+          <t>FR-CH</t>
         </is>
       </c>
       <c r="B26" s="4" t="inlineStr">
         <is>
-          <t>Niederlande</t>
+          <t>Frankreich</t>
         </is>
       </c>
       <c r="C26" s="4" t="inlineStr">
         <is>
-          <t>Frankreich</t>
+          <t>Schweiz</t>
         </is>
       </c>
       <c r="D26" s="6" t="n">
@@ -23200,11 +23201,11 @@
     <row r="6">
       <c r="A6" s="4" t="inlineStr">
         <is>
-          <t>Deutschland</t>
+          <t>Benelux</t>
         </is>
       </c>
       <c r="B6" s="6" t="n">
-        <v>17.39895844079881</v>
+        <v>17.59895844079881</v>
       </c>
       <c r="C6" s="6" t="n"/>
       <c r="D6" s="6" t="n"/>
@@ -23227,11 +23228,11 @@
     <row r="7">
       <c r="A7" s="4" t="inlineStr">
         <is>
-          <t>Frankreich</t>
+          <t>Deutschland</t>
         </is>
       </c>
       <c r="B7" s="6" t="n">
-        <v>17.54895844079881</v>
+        <v>17.39895844079881</v>
       </c>
       <c r="C7" s="6" t="n"/>
       <c r="D7" s="6" t="n"/>
@@ -23254,11 +23255,11 @@
     <row r="8">
       <c r="A8" s="4" t="inlineStr">
         <is>
-          <t>LNG</t>
+          <t>Frankreich</t>
         </is>
       </c>
       <c r="B8" s="6" t="n">
-        <v>17.19895844079881</v>
+        <v>17.54895844079881</v>
       </c>
       <c r="C8" s="6" t="n"/>
       <c r="D8" s="6" t="n"/>
@@ -23281,11 +23282,11 @@
     <row r="9">
       <c r="A9" s="4" t="inlineStr">
         <is>
-          <t>Niederlande</t>
+          <t>LNG</t>
         </is>
       </c>
       <c r="B9" s="6" t="n">
-        <v>17.59895844079881</v>
+        <v>17.19895844079881</v>
       </c>
       <c r="C9" s="6" t="n"/>
       <c r="D9" s="6" t="n"/>
@@ -25315,4 +25316,110 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="28.5703125" customWidth="1" min="1" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="7" t="inlineStr">
+        <is>
+          <t>Master</t>
+        </is>
+      </c>
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>Region</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Deutschland</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Deutschland</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Frankreich</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Frankreich</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Benelux</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Niederlande</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Schweiz</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Schweiz</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Benelux</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Luxemburg</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Benelux</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Benelux</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>